<commit_message>
Deploying to gh-pages from @ codeforIATI/codelists@ac938c2e86ac712d2d31b4494eff601deca28aec 🚀
</commit_message>
<xml_diff>
--- a/api/1/clv2/xlsx/en/SectorCOFOG.xlsx
+++ b/api/1/clv2/xlsx/en/SectorCOFOG.xlsx
@@ -40,15 +40,15 @@
     <t>codeforiati:group-name</t>
   </si>
   <si>
+    <t>codeforiati:cofog-class</t>
+  </si>
+  <si>
+    <t>codeforiati:category-code</t>
+  </si>
+  <si>
     <t>codeforiati:cofog-group</t>
   </si>
   <si>
-    <t>codeforiati:cofog-class</t>
-  </si>
-  <si>
-    <t>codeforiati:category-code</t>
-  </si>
-  <si>
     <t>11110</t>
   </si>
   <si>
@@ -73,15 +73,15 @@
     <t>Education</t>
   </si>
   <si>
+    <t>09.8.0 - Education n.e.c. (CS)</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
     <t>09.8 - Education n.e.c.</t>
   </si>
   <si>
-    <t>09.8.0 - Education n.e.c. (CS)</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
     <t>11120</t>
   </si>
   <si>
@@ -91,12 +91,12 @@
     <t>Educational buildings, equipment, materials; subsidiary services to education (boarding facilities, staff housing); language training; colloquia, seminars, lectures, etc.</t>
   </si>
   <si>
+    <t>09.6.0 - Subsidiary services to education (IS)</t>
+  </si>
+  <si>
     <t>09.6 - Subsidiary services to education</t>
   </si>
   <si>
-    <t>09.6.0 - Subsidiary services to education (IS)</t>
-  </si>
-  <si>
     <t>11130</t>
   </si>
   <si>
@@ -115,12 +115,12 @@
     <t>Research and studies on education effectiveness, relevance and quality; systematic evaluation and monitoring.</t>
   </si>
   <si>
+    <t>09.7.0 - R&amp;D Education (CS)</t>
+  </si>
+  <si>
     <t>09.7 - R&amp;D Education</t>
   </si>
   <si>
-    <t>09.7.0 - R&amp;D Education (CS)</t>
-  </si>
-  <si>
     <t>11220</t>
   </si>
   <si>
@@ -133,15 +133,15 @@
     <t>Basic Education</t>
   </si>
   <si>
+    <t>09.1.2 - Primary education (IS)</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
     <t>09.1 - Pre‐primary and primary education</t>
   </si>
   <si>
-    <t>09.1.2 - Primary education (IS)</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
     <t>11230</t>
   </si>
   <si>
@@ -193,12 +193,12 @@
     <t>07 - Health</t>
   </si>
   <si>
+    <t>07.4.0 - Public health services (IS)</t>
+  </si>
+  <si>
     <t>07.4 - Public health services</t>
   </si>
   <si>
-    <t>07.4.0 - Public health services (IS)</t>
-  </si>
-  <si>
     <t>11260</t>
   </si>
   <si>
@@ -208,12 +208,12 @@
     <t>Second cycle systematic instruction at junior level.</t>
   </si>
   <si>
+    <t>09.2.1 - Lower‐secondary education (IS)</t>
+  </si>
+  <si>
     <t>09.2 - Secondary education</t>
   </si>
   <si>
-    <t>09.2.1 - Lower‐secondary education (IS)</t>
-  </si>
-  <si>
     <t>11320</t>
   </si>
   <si>
@@ -241,12 +241,12 @@
     <t>Elementary vocational training and secondary level technical education; on-the job training; apprenticeships; including informal vocational training.</t>
   </si>
   <si>
+    <t>09.5.0 - Education not definable by level (IS)</t>
+  </si>
+  <si>
     <t>09.5 - Education not definable by level</t>
   </si>
   <si>
-    <t>09.5.0 - Education not definable by level (IS)</t>
-  </si>
-  <si>
     <t>11420</t>
   </si>
   <si>
@@ -259,15 +259,15 @@
     <t>Post-Secondary Education</t>
   </si>
   <si>
+    <t>09.4.1 - First stage of tertiary education (IS)</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
     <t>09.4 - Tertiary education</t>
   </si>
   <si>
-    <t>09.4.1 - First stage of tertiary education (IS)</t>
-  </si>
-  <si>
-    <t>114</t>
-  </si>
-  <si>
     <t>11430</t>
   </si>
   <si>
@@ -277,12 +277,12 @@
     <t>Professional-level vocational training programmes and in-service training.</t>
   </si>
   <si>
+    <t>09.3.0 - Post‐secondary non‐tertiary education (IS)</t>
+  </si>
+  <si>
     <t>09.3 - Post‐secondary non‐tertiary education</t>
   </si>
   <si>
-    <t>09.3.0 - Post‐secondary non‐tertiary education (IS)</t>
-  </si>
-  <si>
     <t>12110</t>
   </si>
   <si>
@@ -301,15 +301,15 @@
     <t>Health</t>
   </si>
   <si>
+    <t>07.6.0 - Health n.e.c. (CS)</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
     <t>07.6 - Health n.e.c.</t>
   </si>
   <si>
-    <t>07.6.0 - Health n.e.c. (CS)</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
     <t>12181</t>
   </si>
   <si>
@@ -328,12 +328,12 @@
     <t>General medical research (excluding basic health research and research for prevention and control of NCDs (12382)).</t>
   </si>
   <si>
+    <t>07.5.0 - R&amp;D Health (CS)</t>
+  </si>
+  <si>
     <t>07.5 - R&amp;D Health</t>
   </si>
   <si>
-    <t>07.5.0 - R&amp;D Health (CS)</t>
-  </si>
-  <si>
     <t>12191</t>
   </si>
   <si>
@@ -343,12 +343,12 @@
     <t>Laboratories, specialised clinics and hospitals (including equipment and supplies); ambulances; dental services; medical rehabilitation. Excludes noncommunicable diseases (123xx).</t>
   </si>
   <si>
+    <t>07.2.1 - General medical services (IS)</t>
+  </si>
+  <si>
     <t>07.2 - Outpatient services</t>
   </si>
   <si>
-    <t>07.2.1 - General medical services (IS)</t>
-  </si>
-  <si>
     <t>12196</t>
   </si>
   <si>
@@ -382,12 +382,12 @@
     <t>District-level hospitals, clinics and dispensaries and related medical equipment; excluding specialised hospitals and clinics (12191).</t>
   </si>
   <si>
+    <t>07.3.1 - General hospital services (IS)</t>
+  </si>
+  <si>
     <t>07.3 - Hospital services</t>
   </si>
   <si>
-    <t>07.3.1 - General hospital services (IS)</t>
-  </si>
-  <si>
     <t>12240</t>
   </si>
   <si>
@@ -589,12 +589,12 @@
     <t>Water Supply &amp; Sanitation</t>
   </si>
   <si>
+    <t>06.3.0 - Water supply (CS)</t>
+  </si>
+  <si>
     <t>06.3 - Water supply</t>
   </si>
   <si>
-    <t>06.3.0 - Water supply (CS)</t>
-  </si>
-  <si>
     <t>14015</t>
   </si>
   <si>
@@ -607,12 +607,12 @@
     <t>05 - Environmental protection</t>
   </si>
   <si>
+    <t>05.6.0 - Environmental protection n.e.c. (CS)</t>
+  </si>
+  <si>
     <t>05.6 - Environmental protection n.e.c.</t>
   </si>
   <si>
-    <t>05.6.0 - Environmental protection n.e.c. (CS)</t>
-  </si>
-  <si>
     <t>14020</t>
   </si>
   <si>
@@ -640,12 +640,12 @@
     <t>Large scale sewerage including trunk sewers and sewage pumping stations; domestic and industrial waste water treatment plants.</t>
   </si>
   <si>
+    <t>05.2.0 - Waste water management (CS)</t>
+  </si>
+  <si>
     <t>05.2 - Waste water management</t>
   </si>
   <si>
-    <t>05.2.0 - Waste water management (CS)</t>
-  </si>
-  <si>
     <t>14030</t>
   </si>
   <si>
@@ -691,12 +691,12 @@
     <t>Municipal and industrial solid waste management, including hazardous and toxic waste; collection, disposal and treatment; landfill areas; composting and reuse.</t>
   </si>
   <si>
+    <t>05.1.0 - Waste management (CS)</t>
+  </si>
+  <si>
     <t>05.1 - Waste management</t>
   </si>
   <si>
-    <t>05.1.0 - Waste management (CS)</t>
-  </si>
-  <si>
     <t>14081</t>
   </si>
   <si>
@@ -727,15 +727,15 @@
     <t>Government &amp; Civil Society</t>
   </si>
   <si>
+    <t>01.3.1 - General personnel services (CS)</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
     <t>01.3 - General services</t>
   </si>
   <si>
-    <t>01.3.1 - General personnel services (CS)</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
     <t>15111</t>
   </si>
   <si>
@@ -745,12 +745,12 @@
     <t>Fiscal policy and planning; support to ministries of finance; strengthening financial and managerial accountability; public expenditure management; improving financial management systems; budget drafting; inter-governmental fiscal relations, public audit, public debt. (Use code 15114 for domestic revenue mobilisation and code 33120 for customs).</t>
   </si>
   <si>
+    <t>01.1.2 - Financial and fiscal affairs (CS)</t>
+  </si>
+  <si>
     <t>01.1 - Executive and legislative organs, financial and fiscal affairs, external affairs</t>
   </si>
   <si>
-    <t>01.1.2 - Financial and fiscal affairs (CS)</t>
-  </si>
-  <si>
     <t>15112</t>
   </si>
   <si>
@@ -760,12 +760,12 @@
     <t>Decentralisation processes (including political, administrative and fiscal dimensions); intergovernmental relations and federalism; strengthening departments of regional and local government, regional and local authorities and their national associations. (Use specific sector codes for decentralisation of sector management and services.)</t>
   </si>
   <si>
+    <t>01.8.0 - Transfers of a general character between different levels of government (CS)</t>
+  </si>
+  <si>
     <t>01.8 - Transfers of a general character between different levels of government</t>
   </si>
   <si>
-    <t>01.8.0 - Transfers of a general character between different levels of government (CS)</t>
-  </si>
-  <si>
     <t>15113</t>
   </si>
   <si>
@@ -778,12 +778,12 @@
     <t>03 - Public order and safety</t>
   </si>
   <si>
+    <t>03.6.0 - Public order and safety n.e.c. (CS)</t>
+  </si>
+  <si>
     <t>03.6 - Public order and safety n.e.c.</t>
   </si>
   <si>
-    <t>03.6.0 - Public order and safety n.e.c. (CS)</t>
-  </si>
-  <si>
     <t>15114</t>
   </si>
   <si>
@@ -859,12 +859,12 @@
     <t>Support to administration of developing countries' foreign aid (including triangular and south-south cooperation).</t>
   </si>
   <si>
+    <t>01.2.2 - Economic aid routed through international organizations (CS)</t>
+  </si>
+  <si>
     <t>01.2 - Foreign economic aid</t>
   </si>
   <si>
-    <t>01.2.2 - Economic aid routed through international organizations (CS)</t>
-  </si>
-  <si>
     <t>15124</t>
   </si>
   <si>
@@ -943,12 +943,12 @@
     <t>Judicial law and order sectors; policy development within ministries of justice or equivalents.</t>
   </si>
   <si>
+    <t>03.3.0 - Law courts (CS)</t>
+  </si>
+  <si>
     <t>03.3 - Law courts</t>
   </si>
   <si>
-    <t>03.3.0 - Law courts (CS)</t>
-  </si>
-  <si>
     <t>15132</t>
   </si>
   <si>
@@ -958,12 +958,12 @@
     <t>Police affairs and services.</t>
   </si>
   <si>
+    <t>03.1.0 - Police services (CS)</t>
+  </si>
+  <si>
     <t>03.1 - Police services</t>
   </si>
   <si>
-    <t>03.1.0 - Police services (CS)</t>
-  </si>
-  <si>
     <t>15133</t>
   </si>
   <si>
@@ -973,12 +973,12 @@
     <t>Fire-prevention and fire-fighting affairs and services.</t>
   </si>
   <si>
+    <t>03.2.0 - Fire‐protection services (CS)</t>
+  </si>
+  <si>
     <t>03.2 - Fire‐protection services</t>
   </si>
   <si>
-    <t>03.2.0 - Fire‐protection services (CS)</t>
-  </si>
-  <si>
     <t>15134</t>
   </si>
   <si>
@@ -1012,12 +1012,12 @@
     <t>Prisons</t>
   </si>
   <si>
+    <t>03.4.0 - Prisons (CS)</t>
+  </si>
+  <si>
     <t>03.4 - Prisons</t>
   </si>
   <si>
-    <t>03.4.0 - Prisons (CS)</t>
-  </si>
-  <si>
     <t>15142</t>
   </si>
   <si>
@@ -1030,12 +1030,12 @@
     <t>04 - Economic affairs</t>
   </si>
   <si>
+    <t>04.1.1 - General economic and commercial affairs (CS)</t>
+  </si>
+  <si>
     <t>04.1 - General economic, commercial and labour affairs</t>
   </si>
   <si>
-    <t>04.1.1 - General economic and commercial affairs (CS)</t>
-  </si>
-  <si>
     <t>15143</t>
   </si>
   <si>
@@ -1072,12 +1072,12 @@
     <t>Electoral management bodies and processes, election observation, voters' education. (Use code 15230 when in the context of an international peacekeeping operation.)</t>
   </si>
   <si>
+    <t>01.6.0 - General public services n.e.c. (CS)</t>
+  </si>
+  <si>
     <t>01.6 - General public services n.e.c.</t>
   </si>
   <si>
-    <t>01.6.0 - General public services n.e.c. (CS)</t>
-  </si>
-  <si>
     <t>15152</t>
   </si>
   <si>
@@ -1099,12 +1099,12 @@
     <t>Activities that support free and uncensored flow of information on public issues; activities that increase the editorial and technical skills and the integrity of the print and broadcast media, e.g. training of journalists. (Use codes 22010-22040 for provision of equipment and capital assistance to media.)</t>
   </si>
   <si>
+    <t>04.6.0 - Communication (CS)</t>
+  </si>
+  <si>
     <t>04.6 - Communication</t>
   </si>
   <si>
-    <t>04.6.0 - Communication (CS)</t>
-  </si>
-  <si>
     <t>15154</t>
   </si>
   <si>
@@ -1150,12 +1150,12 @@
     <t>10 - Social protection</t>
   </si>
   <si>
+    <t>10.7.0 - Social exclusion n.e.c. (IS)</t>
+  </si>
+  <si>
     <t>10.7 - Social exclusion n.e.c.</t>
   </si>
   <si>
-    <t>10.7.0 - Social exclusion n.e.c. (IS)</t>
-  </si>
-  <si>
     <t>15180</t>
   </si>
   <si>
@@ -1192,12 +1192,12 @@
     <t>Collection, production, management and dissemination of statistics and data related to Government &amp; Civil Society. Includes macroeconomic statistics, government finance, fiscal and public sector statistics, support to development of administrative data infrastructure, civil society surveys.</t>
   </si>
   <si>
+    <t>01.5.0 - R&amp;D General public services (CS)</t>
+  </si>
+  <si>
     <t>01.5 - R&amp;D General public services</t>
   </si>
   <si>
-    <t>01.5.0 - R&amp;D General public services (CS)</t>
-  </si>
-  <si>
     <t>15210</t>
   </si>
   <si>
@@ -1234,12 +1234,12 @@
     <t>02 - Defence</t>
   </si>
   <si>
+    <t>02.3.0 - Foreign military aid (CS)</t>
+  </si>
+  <si>
     <t>02.3 - Foreign military aid</t>
   </si>
   <si>
-    <t>02.3.0 - Foreign military aid (CS)</t>
-  </si>
-  <si>
     <t>15240</t>
   </si>
   <si>
@@ -1282,12 +1282,12 @@
     <t>Other Social Infrastructure &amp; Services</t>
   </si>
   <si>
+    <t>10.9.0 - Social protection n.e.c. (CS)</t>
+  </si>
+  <si>
     <t>10.9 - Social protection n.e.c.</t>
   </si>
   <si>
-    <t>10.9.0 - Social protection n.e.c. (CS)</t>
-  </si>
-  <si>
     <t>16011</t>
   </si>
   <si>
@@ -1315,12 +1315,12 @@
     <t>Social protection schemes in the form of cash or in-kind benefits, including pensions, against the risks linked to old age.</t>
   </si>
   <si>
+    <t>10.2.0 - Old age (IS)</t>
+  </si>
+  <si>
     <t>10.2 - Old age</t>
   </si>
   <si>
-    <t>10.2.0 - Old age (IS)</t>
-  </si>
-  <si>
     <t>16014</t>
   </si>
   <si>
@@ -1348,12 +1348,12 @@
     <t>Employment policy and planning; institution capacity building and advice; employment creation and income generation programmes; including activities specifically designed for the needs of vulnerable groups.</t>
   </si>
   <si>
+    <t>10.5.0 - Unemployment (IS)</t>
+  </si>
+  <si>
     <t>10.5 - Unemployment</t>
   </si>
   <si>
-    <t>10.5.0 - Unemployment (IS)</t>
-  </si>
-  <si>
     <t>16030</t>
   </si>
   <si>
@@ -1363,12 +1363,12 @@
     <t>Housing sector policy, planning and programmes; excluding low-cost housing and slum clearance (16040).</t>
   </si>
   <si>
+    <t>06.6.0 - Housing and community amenities n.e.c. (CS)</t>
+  </si>
+  <si>
     <t>06.6 - Housing and community amenities n.e.c.</t>
   </si>
   <si>
-    <t>06.6.0 - Housing and community amenities n.e.c. (CS)</t>
-  </si>
-  <si>
     <t>16040</t>
   </si>
   <si>
@@ -1378,12 +1378,12 @@
     <t>Including slum clearance.</t>
   </si>
   <si>
+    <t>06.1.0 - Housing development (CS)</t>
+  </si>
+  <si>
     <t>06.1 - Housing development</t>
   </si>
   <si>
-    <t>06.1.0 - Housing development (CS)</t>
-  </si>
-  <si>
     <t>16050</t>
   </si>
   <si>
@@ -1405,12 +1405,12 @@
     <t>08 - Recreation, culture and religion</t>
   </si>
   <si>
+    <t>08.2.0 - Cultural services (IS)</t>
+  </si>
+  <si>
     <t>08.2 - Cultural services</t>
   </si>
   <si>
-    <t>08.2.0 - Cultural services (IS)</t>
-  </si>
-  <si>
     <t>16062</t>
   </si>
   <si>
@@ -1444,12 +1444,12 @@
     <t>Recreation and sport</t>
   </si>
   <si>
+    <t>08.1.0 - Recreational and sporting services (IS)</t>
+  </si>
+  <si>
     <t>08.1 - Recreational and sporting services</t>
   </si>
   <si>
-    <t>08.1.0 - Recreational and sporting services (IS)</t>
-  </si>
-  <si>
     <t>16066</t>
   </si>
   <si>
@@ -1528,12 +1528,12 @@
     <t>Road infrastructure, road vehicles; passenger road transport, motor passenger cars.</t>
   </si>
   <si>
+    <t>04.5.1 - Road transport (CS)</t>
+  </si>
+  <si>
     <t>04.5 - Transport</t>
   </si>
   <si>
-    <t>04.5.1 - Road transport (CS)</t>
-  </si>
-  <si>
     <t>21021</t>
   </si>
   <si>
@@ -1615,12 +1615,12 @@
     <t>Whether or not related to transportation. Whenever possible, report storage projects under the sector of the resource being stored.</t>
   </si>
   <si>
+    <t>04.7.1 - Distributive trades, storage and warehousing (CS)</t>
+  </si>
+  <si>
     <t>04.7 - Other industries</t>
   </si>
   <si>
-    <t>04.7.1 - Distributive trades, storage and warehousing (CS)</t>
-  </si>
-  <si>
     <t>21081</t>
   </si>
   <si>
@@ -1684,12 +1684,12 @@
     <t>Radio and TV links, equipment; newspapers; printing and publishing.</t>
   </si>
   <si>
+    <t>08.3.0 - Broadcasting and publishing services (CS)</t>
+  </si>
+  <si>
     <t>08.3 - Broadcasting and publishing services</t>
   </si>
   <si>
-    <t>08.3.0 - Broadcasting and publishing services (CS)</t>
-  </si>
-  <si>
     <t>22040</t>
   </si>
   <si>
@@ -1717,15 +1717,15 @@
     <t>Energy</t>
   </si>
   <si>
+    <t>04.3.5 - Electricity (CS)</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
     <t>04.3 - Fuel and energy</t>
   </si>
   <si>
-    <t>04.3.5 - Electricity (CS)</t>
-  </si>
-  <si>
-    <t>231</t>
-  </si>
-  <si>
     <t>23111</t>
   </si>
   <si>
@@ -1741,12 +1741,12 @@
     <t>Regulation of the energy sector, including wholesale and retail electricity provision.</t>
   </si>
   <si>
+    <t>04.8.3 - R&amp;D Fuel and energy (CS)</t>
+  </si>
+  <si>
     <t>04.8 - R&amp;D Economic affairs</t>
   </si>
   <si>
-    <t>04.8.3 - R&amp;D Fuel and energy (CS)</t>
-  </si>
-  <si>
     <t>23181</t>
   </si>
   <si>
@@ -2140,15 +2140,15 @@
     <t>Agriculture, Forestry, Fishing</t>
   </si>
   <si>
+    <t>04.2.1 - Agriculture (CS)</t>
+  </si>
+  <si>
+    <t>311</t>
+  </si>
+  <si>
     <t>04.2 - Agriculture, forestry, fishing and hunting</t>
   </si>
   <si>
-    <t>04.2.1 - Agriculture (CS)</t>
-  </si>
-  <si>
-    <t>311</t>
-  </si>
-  <si>
     <t>31120</t>
   </si>
   <si>
@@ -2428,15 +2428,15 @@
     <t>Industry, Mining, Construction</t>
   </si>
   <si>
+    <t>04.4.2 - Manufacturing (CS)</t>
+  </si>
+  <si>
+    <t>321</t>
+  </si>
+  <si>
     <t>04.4 - Mining, manufacturing and construction</t>
   </si>
   <si>
-    <t>04.4.2 - Manufacturing (CS)</t>
-  </si>
-  <si>
-    <t>321</t>
-  </si>
-  <si>
     <t>32120</t>
   </si>
   <si>
@@ -2812,12 +2812,12 @@
     <t>Including natural reserves and actions in the surrounding areas; other measures to protect endangered or vulnerable species and their habitats (e.g. wetlands preservation).</t>
   </si>
   <si>
+    <t>05.4.0 - Protection of biodiversity and landscape (CS)</t>
+  </si>
+  <si>
     <t>05.4 - Protection of biodiversity and landscape</t>
   </si>
   <si>
-    <t>05.4.0 - Protection of biodiversity and landscape (CS)</t>
-  </si>
-  <si>
     <t>41040</t>
   </si>
   <si>
@@ -2854,12 +2854,12 @@
     <t>Other Multisector</t>
   </si>
   <si>
+    <t>04.9.0 - Economic affairs n.e.c. (CS)</t>
+  </si>
+  <si>
     <t>04.9 - Economic affairs n.e.c.</t>
   </si>
   <si>
-    <t>04.9.0 - Economic affairs n.e.c. (CS)</t>
-  </si>
-  <si>
     <t>43030</t>
   </si>
   <si>
@@ -2878,12 +2878,12 @@
     <t>Urban development and planning; urban management, land information systems.</t>
   </si>
   <si>
+    <t>06.2.0 - Community development (CS)</t>
+  </si>
+  <si>
     <t>06.2 - Community development</t>
   </si>
   <si>
-    <t>06.2.0 - Community development (CS)</t>
-  </si>
-  <si>
     <t>43032</t>
   </si>
   <si>
@@ -2935,12 +2935,12 @@
     <t>Disaster risk reduction activities if not sector specific. Comprises risk assessments, structural prevention measures (e.g. flood prevention infrastructure), preparedness measures (e.g. early warning systems) normative prevention measures (e.g. building codes, land-use planning), and risk transfer systems (e.g. insurance schemes, risk funds). Also includes building local and national capacities and supporting the establishment of efficient and sustainable national structures able to promote disaster risk reduction.</t>
   </si>
   <si>
+    <t>02.2.0 - Civil defence (CS)</t>
+  </si>
+  <si>
     <t>02.2 - Civil defence</t>
   </si>
   <si>
-    <t>02.2.0 - Civil defence (CS)</t>
-  </si>
-  <si>
     <t>43071</t>
   </si>
   <si>
@@ -2959,12 +2959,12 @@
     <t>Short or longer term household food security programmes and activities that improve the access of households to nutritionally adequate diets (excluding any cash transfers within broader social welfare programmes that do not have a specific food security, food acquisition or nutrition focus which should be reported under code 16010).</t>
   </si>
   <si>
+    <t>10.4.0 - Family and children (IS)</t>
+  </si>
+  <si>
     <t>10.4 - Family and children</t>
   </si>
   <si>
-    <t>10.4.0 - Family and children (IS)</t>
-  </si>
-  <si>
     <t>43073</t>
   </si>
   <si>
@@ -2992,12 +2992,12 @@
     <t>When sector cannot be identified.</t>
   </si>
   <si>
+    <t>01.4.0 - Basic research (CS)</t>
+  </si>
+  <si>
     <t>01.4 - Basic research</t>
   </si>
   <si>
-    <t>01.4.0 - Basic research (CS)</t>
-  </si>
-  <si>
     <t>51010</t>
   </si>
   <si>
@@ -3067,10 +3067,10 @@
     <t>Action Relating to Debt</t>
   </si>
   <si>
+    <t>01.7.0 - Public debt transactions (CS)</t>
+  </si>
+  <si>
     <t>01.7 - Public debt transactions</t>
-  </si>
-  <si>
-    <t>01.7.0 - Public debt transactions (CS)</t>
   </si>
   <si>
     <t>60020</t>
@@ -3759,10 +3759,10 @@
         <v>25</v>
       </c>
       <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
         <v>26</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3829,10 +3829,10 @@
         <v>33</v>
       </c>
       <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
         <v>34</v>
-      </c>
-      <c r="K5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -3899,10 +3899,10 @@
         <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -4001,10 +4001,10 @@
         <v>18</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="J10" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="K10" t="s">
         <v>41</v>
@@ -4039,10 +4039,10 @@
         <v>59</v>
       </c>
       <c r="J11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" t="s">
         <v>60</v>
-      </c>
-      <c r="K11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -4074,10 +4074,10 @@
         <v>64</v>
       </c>
       <c r="J12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" t="s">
         <v>65</v>
-      </c>
-      <c r="K12" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -4106,13 +4106,13 @@
         <v>18</v>
       </c>
       <c r="I13" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="J13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K13" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -4144,10 +4144,10 @@
         <v>75</v>
       </c>
       <c r="J14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" t="s">
         <v>76</v>
-      </c>
-      <c r="K14" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -4214,10 +4214,10 @@
         <v>87</v>
       </c>
       <c r="J16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" t="s">
         <v>88</v>
-      </c>
-      <c r="K16" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -4319,10 +4319,10 @@
         <v>104</v>
       </c>
       <c r="J19" t="s">
+        <v>96</v>
+      </c>
+      <c r="K19" t="s">
         <v>105</v>
-      </c>
-      <c r="K19" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -4354,10 +4354,10 @@
         <v>109</v>
       </c>
       <c r="J20" t="s">
+        <v>96</v>
+      </c>
+      <c r="K20" t="s">
         <v>110</v>
-      </c>
-      <c r="K20" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -4424,10 +4424,10 @@
         <v>59</v>
       </c>
       <c r="J22" t="s">
+        <v>118</v>
+      </c>
+      <c r="K22" t="s">
         <v>60</v>
-      </c>
-      <c r="K22" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -4459,10 +4459,10 @@
         <v>122</v>
       </c>
       <c r="J23" t="s">
+        <v>118</v>
+      </c>
+      <c r="K23" t="s">
         <v>123</v>
-      </c>
-      <c r="K23" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -4494,10 +4494,10 @@
         <v>59</v>
       </c>
       <c r="J24" t="s">
+        <v>118</v>
+      </c>
+      <c r="K24" t="s">
         <v>60</v>
-      </c>
-      <c r="K24" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -4529,10 +4529,10 @@
         <v>59</v>
       </c>
       <c r="J25" t="s">
+        <v>118</v>
+      </c>
+      <c r="K25" t="s">
         <v>60</v>
-      </c>
-      <c r="K25" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -4564,10 +4564,10 @@
         <v>59</v>
       </c>
       <c r="J26" t="s">
+        <v>118</v>
+      </c>
+      <c r="K26" t="s">
         <v>60</v>
-      </c>
-      <c r="K26" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -4599,10 +4599,10 @@
         <v>59</v>
       </c>
       <c r="J27" t="s">
+        <v>118</v>
+      </c>
+      <c r="K27" t="s">
         <v>60</v>
-      </c>
-      <c r="K27" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -4634,10 +4634,10 @@
         <v>59</v>
       </c>
       <c r="J28" t="s">
+        <v>118</v>
+      </c>
+      <c r="K28" t="s">
         <v>60</v>
-      </c>
-      <c r="K28" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -4669,10 +4669,10 @@
         <v>59</v>
       </c>
       <c r="J29" t="s">
+        <v>118</v>
+      </c>
+      <c r="K29" t="s">
         <v>60</v>
-      </c>
-      <c r="K29" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -4704,10 +4704,10 @@
         <v>95</v>
       </c>
       <c r="J30" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="K30" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -4739,10 +4739,10 @@
         <v>59</v>
       </c>
       <c r="J31" t="s">
+        <v>149</v>
+      </c>
+      <c r="K31" t="s">
         <v>60</v>
-      </c>
-      <c r="K31" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -4774,10 +4774,10 @@
         <v>59</v>
       </c>
       <c r="J32" t="s">
+        <v>149</v>
+      </c>
+      <c r="K32" t="s">
         <v>60</v>
-      </c>
-      <c r="K32" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -4809,10 +4809,10 @@
         <v>59</v>
       </c>
       <c r="J33" t="s">
+        <v>149</v>
+      </c>
+      <c r="K33" t="s">
         <v>60</v>
-      </c>
-      <c r="K33" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -4844,10 +4844,10 @@
         <v>59</v>
       </c>
       <c r="J34" t="s">
+        <v>149</v>
+      </c>
+      <c r="K34" t="s">
         <v>60</v>
-      </c>
-      <c r="K34" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -4879,10 +4879,10 @@
         <v>59</v>
       </c>
       <c r="J35" t="s">
+        <v>149</v>
+      </c>
+      <c r="K35" t="s">
         <v>60</v>
-      </c>
-      <c r="K35" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -4914,10 +4914,10 @@
         <v>104</v>
       </c>
       <c r="J36" t="s">
+        <v>149</v>
+      </c>
+      <c r="K36" t="s">
         <v>105</v>
-      </c>
-      <c r="K36" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -4945,7 +4945,7 @@
       <c r="I37" t="s">
         <v>59</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4974,7 +4974,7 @@
       <c r="I38" t="s">
         <v>59</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
         <v>60</v>
       </c>
     </row>
@@ -5003,7 +5003,7 @@
       <c r="I39" t="s">
         <v>59</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>60</v>
       </c>
     </row>
@@ -5032,7 +5032,7 @@
       <c r="I40" t="s">
         <v>59</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>60</v>
       </c>
     </row>
@@ -5061,8 +5061,8 @@
       <c r="I41" t="s">
         <v>95</v>
       </c>
-      <c r="J41" t="s">
-        <v>96</v>
+      <c r="K41" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -5090,7 +5090,7 @@
       <c r="I42" t="s">
         <v>104</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>105</v>
       </c>
     </row>
@@ -5119,7 +5119,7 @@
       <c r="I43" t="s">
         <v>191</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5148,7 +5148,7 @@
       <c r="I44" t="s">
         <v>197</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
         <v>198</v>
       </c>
     </row>
@@ -5177,7 +5177,7 @@
       <c r="I45" t="s">
         <v>191</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5206,7 +5206,7 @@
       <c r="I46" t="s">
         <v>191</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5235,7 +5235,7 @@
       <c r="I47" t="s">
         <v>208</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>209</v>
       </c>
     </row>
@@ -5264,7 +5264,7 @@
       <c r="I48" t="s">
         <v>191</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5293,7 +5293,7 @@
       <c r="I49" t="s">
         <v>191</v>
       </c>
-      <c r="J49" t="s">
+      <c r="K49" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5322,7 +5322,7 @@
       <c r="I50" t="s">
         <v>208</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>209</v>
       </c>
     </row>
@@ -5351,7 +5351,7 @@
       <c r="I51" t="s">
         <v>191</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5380,7 +5380,7 @@
       <c r="I52" t="s">
         <v>225</v>
       </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>226</v>
       </c>
     </row>
@@ -5409,8 +5409,8 @@
       <c r="I53" t="s">
         <v>19</v>
       </c>
-      <c r="J53" t="s">
-        <v>20</v>
+      <c r="K53" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -5477,10 +5477,10 @@
         <v>243</v>
       </c>
       <c r="J55" t="s">
+        <v>238</v>
+      </c>
+      <c r="K55" t="s">
         <v>244</v>
-      </c>
-      <c r="K55" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -5512,10 +5512,10 @@
         <v>248</v>
       </c>
       <c r="J56" t="s">
+        <v>238</v>
+      </c>
+      <c r="K56" t="s">
         <v>249</v>
-      </c>
-      <c r="K56" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -5547,10 +5547,10 @@
         <v>254</v>
       </c>
       <c r="J57" t="s">
+        <v>238</v>
+      </c>
+      <c r="K57" t="s">
         <v>255</v>
-      </c>
-      <c r="K57" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -5582,10 +5582,10 @@
         <v>243</v>
       </c>
       <c r="J58" t="s">
+        <v>238</v>
+      </c>
+      <c r="K58" t="s">
         <v>244</v>
-      </c>
-      <c r="K58" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -5617,10 +5617,10 @@
         <v>243</v>
       </c>
       <c r="J59" t="s">
+        <v>238</v>
+      </c>
+      <c r="K59" t="s">
         <v>244</v>
-      </c>
-      <c r="K59" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -5652,10 +5652,10 @@
         <v>243</v>
       </c>
       <c r="J60" t="s">
+        <v>238</v>
+      </c>
+      <c r="K60" t="s">
         <v>244</v>
-      </c>
-      <c r="K60" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -5687,10 +5687,10 @@
         <v>243</v>
       </c>
       <c r="J61" t="s">
+        <v>238</v>
+      </c>
+      <c r="K61" t="s">
         <v>244</v>
-      </c>
-      <c r="K61" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -5722,10 +5722,10 @@
         <v>243</v>
       </c>
       <c r="J62" t="s">
+        <v>238</v>
+      </c>
+      <c r="K62" t="s">
         <v>244</v>
-      </c>
-      <c r="K62" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -5754,13 +5754,13 @@
         <v>236</v>
       </c>
       <c r="I63" t="s">
-        <v>243</v>
+        <v>274</v>
       </c>
       <c r="J63" t="s">
-        <v>274</v>
+        <v>238</v>
       </c>
       <c r="K63" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -5789,13 +5789,13 @@
         <v>236</v>
       </c>
       <c r="I64" t="s">
-        <v>243</v>
+        <v>274</v>
       </c>
       <c r="J64" t="s">
-        <v>274</v>
+        <v>238</v>
       </c>
       <c r="K64" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -5827,10 +5827,10 @@
         <v>281</v>
       </c>
       <c r="J65" t="s">
+        <v>238</v>
+      </c>
+      <c r="K65" t="s">
         <v>282</v>
-      </c>
-      <c r="K65" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -5897,10 +5897,10 @@
         <v>243</v>
       </c>
       <c r="J67" t="s">
+        <v>238</v>
+      </c>
+      <c r="K67" t="s">
         <v>244</v>
-      </c>
-      <c r="K67" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -5929,10 +5929,10 @@
         <v>236</v>
       </c>
       <c r="I68" t="s">
-        <v>237</v>
+        <v>292</v>
       </c>
       <c r="J68" t="s">
-        <v>292</v>
+        <v>238</v>
       </c>
       <c r="K68" t="s">
         <v>239</v>
@@ -5964,10 +5964,10 @@
         <v>236</v>
       </c>
       <c r="I69" t="s">
-        <v>237</v>
+        <v>296</v>
       </c>
       <c r="J69" t="s">
-        <v>296</v>
+        <v>238</v>
       </c>
       <c r="K69" t="s">
         <v>239</v>
@@ -6002,10 +6002,10 @@
         <v>248</v>
       </c>
       <c r="J70" t="s">
+        <v>238</v>
+      </c>
+      <c r="K70" t="s">
         <v>249</v>
-      </c>
-      <c r="K70" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -6037,10 +6037,10 @@
         <v>248</v>
       </c>
       <c r="J71" t="s">
+        <v>238</v>
+      </c>
+      <c r="K71" t="s">
         <v>249</v>
-      </c>
-      <c r="K71" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -6107,10 +6107,10 @@
         <v>309</v>
       </c>
       <c r="J73" t="s">
+        <v>238</v>
+      </c>
+      <c r="K73" t="s">
         <v>310</v>
-      </c>
-      <c r="K73" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -6142,10 +6142,10 @@
         <v>314</v>
       </c>
       <c r="J74" t="s">
+        <v>238</v>
+      </c>
+      <c r="K74" t="s">
         <v>315</v>
-      </c>
-      <c r="K74" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -6177,10 +6177,10 @@
         <v>319</v>
       </c>
       <c r="J75" t="s">
+        <v>238</v>
+      </c>
+      <c r="K75" t="s">
         <v>320</v>
-      </c>
-      <c r="K75" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -6212,10 +6212,10 @@
         <v>309</v>
       </c>
       <c r="J76" t="s">
+        <v>238</v>
+      </c>
+      <c r="K76" t="s">
         <v>310</v>
-      </c>
-      <c r="K76" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -6247,10 +6247,10 @@
         <v>309</v>
       </c>
       <c r="J77" t="s">
+        <v>238</v>
+      </c>
+      <c r="K77" t="s">
         <v>310</v>
-      </c>
-      <c r="K77" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -6282,10 +6282,10 @@
         <v>314</v>
       </c>
       <c r="J78" t="s">
+        <v>238</v>
+      </c>
+      <c r="K78" t="s">
         <v>315</v>
-      </c>
-      <c r="K78" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -6314,10 +6314,10 @@
         <v>332</v>
       </c>
       <c r="J79" t="s">
+        <v>238</v>
+      </c>
+      <c r="K79" t="s">
         <v>333</v>
-      </c>
-      <c r="K79" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -6349,10 +6349,10 @@
         <v>338</v>
       </c>
       <c r="J80" t="s">
+        <v>238</v>
+      </c>
+      <c r="K80" t="s">
         <v>339</v>
-      </c>
-      <c r="K80" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -6384,10 +6384,10 @@
         <v>338</v>
       </c>
       <c r="J81" t="s">
+        <v>238</v>
+      </c>
+      <c r="K81" t="s">
         <v>339</v>
-      </c>
-      <c r="K81" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -6419,10 +6419,10 @@
         <v>338</v>
       </c>
       <c r="J82" t="s">
+        <v>238</v>
+      </c>
+      <c r="K82" t="s">
         <v>339</v>
-      </c>
-      <c r="K82" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -6451,10 +6451,10 @@
         <v>236</v>
       </c>
       <c r="I83" t="s">
-        <v>237</v>
+        <v>296</v>
       </c>
       <c r="J83" t="s">
-        <v>296</v>
+        <v>238</v>
       </c>
       <c r="K83" t="s">
         <v>239</v>
@@ -6489,10 +6489,10 @@
         <v>352</v>
       </c>
       <c r="J84" t="s">
+        <v>238</v>
+      </c>
+      <c r="K84" t="s">
         <v>353</v>
-      </c>
-      <c r="K84" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -6521,13 +6521,13 @@
         <v>236</v>
       </c>
       <c r="I85" t="s">
-        <v>243</v>
+        <v>357</v>
       </c>
       <c r="J85" t="s">
-        <v>357</v>
+        <v>238</v>
       </c>
       <c r="K85" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -6559,10 +6559,10 @@
         <v>361</v>
       </c>
       <c r="J86" t="s">
+        <v>238</v>
+      </c>
+      <c r="K86" t="s">
         <v>362</v>
-      </c>
-      <c r="K86" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -6591,13 +6591,13 @@
         <v>236</v>
       </c>
       <c r="I87" t="s">
-        <v>243</v>
+        <v>357</v>
       </c>
       <c r="J87" t="s">
-        <v>357</v>
+        <v>238</v>
       </c>
       <c r="K87" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -6626,10 +6626,10 @@
         <v>243</v>
       </c>
       <c r="J88" t="s">
+        <v>238</v>
+      </c>
+      <c r="K88" t="s">
         <v>244</v>
-      </c>
-      <c r="K88" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -6661,10 +6661,10 @@
         <v>243</v>
       </c>
       <c r="J89" t="s">
+        <v>238</v>
+      </c>
+      <c r="K89" t="s">
         <v>244</v>
-      </c>
-      <c r="K89" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -6696,10 +6696,10 @@
         <v>254</v>
       </c>
       <c r="J90" t="s">
+        <v>238</v>
+      </c>
+      <c r="K90" t="s">
         <v>255</v>
-      </c>
-      <c r="K90" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -6731,10 +6731,10 @@
         <v>378</v>
       </c>
       <c r="J91" t="s">
+        <v>238</v>
+      </c>
+      <c r="K91" t="s">
         <v>379</v>
-      </c>
-      <c r="K91" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -6766,10 +6766,10 @@
         <v>254</v>
       </c>
       <c r="J92" t="s">
+        <v>238</v>
+      </c>
+      <c r="K92" t="s">
         <v>255</v>
-      </c>
-      <c r="K92" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -6801,10 +6801,10 @@
         <v>248</v>
       </c>
       <c r="J93" t="s">
+        <v>238</v>
+      </c>
+      <c r="K93" t="s">
         <v>249</v>
-      </c>
-      <c r="K93" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -6836,10 +6836,10 @@
         <v>254</v>
       </c>
       <c r="J94" t="s">
+        <v>238</v>
+      </c>
+      <c r="K94" t="s">
         <v>255</v>
-      </c>
-      <c r="K94" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -6871,10 +6871,10 @@
         <v>392</v>
       </c>
       <c r="J95" t="s">
+        <v>238</v>
+      </c>
+      <c r="K95" t="s">
         <v>393</v>
-      </c>
-      <c r="K95" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -6906,10 +6906,10 @@
         <v>254</v>
       </c>
       <c r="J96" t="s">
+        <v>398</v>
+      </c>
+      <c r="K96" t="s">
         <v>255</v>
-      </c>
-      <c r="K96" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -6941,10 +6941,10 @@
         <v>254</v>
       </c>
       <c r="J97" t="s">
+        <v>398</v>
+      </c>
+      <c r="K97" t="s">
         <v>255</v>
-      </c>
-      <c r="K97" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -6976,10 +6976,10 @@
         <v>406</v>
       </c>
       <c r="J98" t="s">
+        <v>398</v>
+      </c>
+      <c r="K98" t="s">
         <v>407</v>
-      </c>
-      <c r="K98" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -7011,10 +7011,10 @@
         <v>254</v>
       </c>
       <c r="J99" t="s">
+        <v>398</v>
+      </c>
+      <c r="K99" t="s">
         <v>255</v>
-      </c>
-      <c r="K99" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -7046,10 +7046,10 @@
         <v>319</v>
       </c>
       <c r="J100" t="s">
+        <v>398</v>
+      </c>
+      <c r="K100" t="s">
         <v>320</v>
-      </c>
-      <c r="K100" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -7081,10 +7081,10 @@
         <v>254</v>
       </c>
       <c r="J101" t="s">
+        <v>398</v>
+      </c>
+      <c r="K101" t="s">
         <v>255</v>
-      </c>
-      <c r="K101" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="102" spans="1:11">
@@ -7112,7 +7112,7 @@
       <c r="I102" t="s">
         <v>422</v>
       </c>
-      <c r="J102" t="s">
+      <c r="K102" t="s">
         <v>423</v>
       </c>
     </row>
@@ -7141,7 +7141,7 @@
       <c r="I103" t="s">
         <v>422</v>
       </c>
-      <c r="J103" t="s">
+      <c r="K103" t="s">
         <v>423</v>
       </c>
     </row>
@@ -7170,7 +7170,7 @@
       <c r="I104" t="s">
         <v>422</v>
       </c>
-      <c r="J104" t="s">
+      <c r="K104" t="s">
         <v>423</v>
       </c>
     </row>
@@ -7199,7 +7199,7 @@
       <c r="I105" t="s">
         <v>433</v>
       </c>
-      <c r="J105" t="s">
+      <c r="K105" t="s">
         <v>434</v>
       </c>
     </row>
@@ -7228,7 +7228,7 @@
       <c r="I106" t="s">
         <v>422</v>
       </c>
-      <c r="J106" t="s">
+      <c r="K106" t="s">
         <v>423</v>
       </c>
     </row>
@@ -7257,7 +7257,7 @@
       <c r="I107" t="s">
         <v>378</v>
       </c>
-      <c r="J107" t="s">
+      <c r="K107" t="s">
         <v>379</v>
       </c>
     </row>
@@ -7286,7 +7286,7 @@
       <c r="I108" t="s">
         <v>444</v>
       </c>
-      <c r="J108" t="s">
+      <c r="K108" t="s">
         <v>445</v>
       </c>
     </row>
@@ -7315,7 +7315,7 @@
       <c r="I109" t="s">
         <v>449</v>
       </c>
-      <c r="J109" t="s">
+      <c r="K109" t="s">
         <v>450</v>
       </c>
     </row>
@@ -7344,7 +7344,7 @@
       <c r="I110" t="s">
         <v>454</v>
       </c>
-      <c r="J110" t="s">
+      <c r="K110" t="s">
         <v>455</v>
       </c>
     </row>
@@ -7373,7 +7373,7 @@
       <c r="I111" t="s">
         <v>422</v>
       </c>
-      <c r="J111" t="s">
+      <c r="K111" t="s">
         <v>423</v>
       </c>
     </row>
@@ -7402,11 +7402,11 @@
       <c r="I112" t="s">
         <v>463</v>
       </c>
-      <c r="J112" t="s">
+      <c r="K112" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:11">
       <c r="A113" t="s">
         <v>465</v>
       </c>
@@ -7429,13 +7429,13 @@
         <v>421</v>
       </c>
       <c r="I113" t="s">
-        <v>237</v>
-      </c>
-      <c r="J113" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="114" spans="1:10">
+      <c r="K113" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="A114" t="s">
         <v>468</v>
       </c>
@@ -7460,11 +7460,11 @@
       <c r="I114" t="s">
         <v>314</v>
       </c>
-      <c r="J114" t="s">
+      <c r="K114" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:11">
       <c r="A115" t="s">
         <v>471</v>
       </c>
@@ -7489,11 +7489,11 @@
       <c r="I115" t="s">
         <v>378</v>
       </c>
-      <c r="J115" t="s">
+      <c r="K115" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:11">
       <c r="A116" t="s">
         <v>474</v>
       </c>
@@ -7515,11 +7515,11 @@
       <c r="I116" t="s">
         <v>476</v>
       </c>
-      <c r="J116" t="s">
+      <c r="K116" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:11">
       <c r="A117" t="s">
         <v>478</v>
       </c>
@@ -7541,11 +7541,11 @@
       <c r="I117" t="s">
         <v>463</v>
       </c>
-      <c r="J117" t="s">
+      <c r="K117" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:11">
       <c r="A118" t="s">
         <v>480</v>
       </c>
@@ -7568,13 +7568,13 @@
         <v>421</v>
       </c>
       <c r="I118" t="s">
-        <v>338</v>
-      </c>
-      <c r="J118" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="119" spans="1:10">
+      <c r="K118" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119" t="s">
         <v>484</v>
       </c>
@@ -7599,11 +7599,11 @@
       <c r="I119" t="s">
         <v>378</v>
       </c>
-      <c r="J119" t="s">
+      <c r="K119" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:11">
       <c r="A120" t="s">
         <v>487</v>
       </c>
@@ -7628,11 +7628,11 @@
       <c r="I120" t="s">
         <v>352</v>
       </c>
-      <c r="J120" t="s">
+      <c r="K120" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:11">
       <c r="A121" t="s">
         <v>492</v>
       </c>
@@ -7655,13 +7655,13 @@
         <v>491</v>
       </c>
       <c r="I121" t="s">
-        <v>237</v>
-      </c>
-      <c r="J121" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="122" spans="1:10">
+      <c r="K121" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122" t="s">
         <v>495</v>
       </c>
@@ -7686,11 +7686,11 @@
       <c r="I122" t="s">
         <v>352</v>
       </c>
-      <c r="J122" t="s">
+      <c r="K122" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:11">
       <c r="A123" t="s">
         <v>498</v>
       </c>
@@ -7715,11 +7715,11 @@
       <c r="I123" t="s">
         <v>352</v>
       </c>
-      <c r="J123" t="s">
+      <c r="K123" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:11">
       <c r="A124" t="s">
         <v>501</v>
       </c>
@@ -7744,11 +7744,11 @@
       <c r="I124" t="s">
         <v>504</v>
       </c>
-      <c r="J124" t="s">
+      <c r="K124" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:11">
       <c r="A125" t="s">
         <v>506</v>
       </c>
@@ -7773,11 +7773,11 @@
       <c r="I125" t="s">
         <v>504</v>
       </c>
-      <c r="J125" t="s">
+      <c r="K125" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:11">
       <c r="A126" t="s">
         <v>509</v>
       </c>
@@ -7802,11 +7802,11 @@
       <c r="I126" t="s">
         <v>504</v>
       </c>
-      <c r="J126" t="s">
+      <c r="K126" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:11">
       <c r="A127" t="s">
         <v>512</v>
       </c>
@@ -7831,11 +7831,11 @@
       <c r="I127" t="s">
         <v>504</v>
       </c>
-      <c r="J127" t="s">
+      <c r="K127" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:11">
       <c r="A128" t="s">
         <v>515</v>
       </c>
@@ -7860,7 +7860,7 @@
       <c r="I128" t="s">
         <v>504</v>
       </c>
-      <c r="J128" t="s">
+      <c r="K128" t="s">
         <v>505</v>
       </c>
     </row>
@@ -7887,10 +7887,10 @@
         <v>491</v>
       </c>
       <c r="I129" t="s">
-        <v>504</v>
-      </c>
-      <c r="J129" t="s">
         <v>521</v>
+      </c>
+      <c r="K129" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="130" spans="1:11">
@@ -7916,10 +7916,10 @@
         <v>491</v>
       </c>
       <c r="I130" t="s">
-        <v>504</v>
-      </c>
-      <c r="J130" t="s">
         <v>525</v>
+      </c>
+      <c r="K130" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="131" spans="1:11">
@@ -7945,10 +7945,10 @@
         <v>491</v>
       </c>
       <c r="I131" t="s">
-        <v>504</v>
-      </c>
-      <c r="J131" t="s">
         <v>529</v>
+      </c>
+      <c r="K131" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="132" spans="1:11">
@@ -7976,7 +7976,7 @@
       <c r="I132" t="s">
         <v>533</v>
       </c>
-      <c r="J132" t="s">
+      <c r="K132" t="s">
         <v>534</v>
       </c>
     </row>
@@ -8002,7 +8002,7 @@
       <c r="I133" t="s">
         <v>392</v>
       </c>
-      <c r="J133" t="s">
+      <c r="K133" t="s">
         <v>393</v>
       </c>
     </row>
@@ -8031,7 +8031,7 @@
       <c r="I134" t="s">
         <v>361</v>
       </c>
-      <c r="J134" t="s">
+      <c r="K134" t="s">
         <v>362</v>
       </c>
     </row>
@@ -8057,7 +8057,7 @@
       <c r="I135" t="s">
         <v>361</v>
       </c>
-      <c r="J135" t="s">
+      <c r="K135" t="s">
         <v>362</v>
       </c>
     </row>
@@ -8086,7 +8086,7 @@
       <c r="I136" t="s">
         <v>361</v>
       </c>
-      <c r="J136" t="s">
+      <c r="K136" t="s">
         <v>362</v>
       </c>
     </row>
@@ -8115,7 +8115,7 @@
       <c r="I137" t="s">
         <v>361</v>
       </c>
-      <c r="J137" t="s">
+      <c r="K137" t="s">
         <v>362</v>
       </c>
     </row>
@@ -8144,7 +8144,7 @@
       <c r="I138" t="s">
         <v>361</v>
       </c>
-      <c r="J138" t="s">
+      <c r="K138" t="s">
         <v>362</v>
       </c>
     </row>
@@ -8173,7 +8173,7 @@
       <c r="I139" t="s">
         <v>556</v>
       </c>
-      <c r="J139" t="s">
+      <c r="K139" t="s">
         <v>557</v>
       </c>
     </row>
@@ -8202,7 +8202,7 @@
       <c r="I140" t="s">
         <v>361</v>
       </c>
-      <c r="J140" t="s">
+      <c r="K140" t="s">
         <v>362</v>
       </c>
     </row>
@@ -8302,10 +8302,10 @@
         <v>575</v>
       </c>
       <c r="J143" t="s">
+        <v>568</v>
+      </c>
+      <c r="K143" t="s">
         <v>576</v>
-      </c>
-      <c r="K143" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="144" spans="1:11">
@@ -8337,10 +8337,10 @@
         <v>575</v>
       </c>
       <c r="J144" t="s">
+        <v>568</v>
+      </c>
+      <c r="K144" t="s">
         <v>576</v>
-      </c>
-      <c r="K144" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="145" spans="1:11">
@@ -8372,10 +8372,10 @@
         <v>575</v>
       </c>
       <c r="J145" t="s">
+        <v>568</v>
+      </c>
+      <c r="K145" t="s">
         <v>576</v>
-      </c>
-      <c r="K145" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="146" spans="1:11">
@@ -8442,10 +8442,10 @@
         <v>567</v>
       </c>
       <c r="J147" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="K147" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
     </row>
     <row r="148" spans="1:11">
@@ -8477,10 +8477,10 @@
         <v>567</v>
       </c>
       <c r="J148" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="K148" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
     </row>
     <row r="149" spans="1:11">
@@ -8512,10 +8512,10 @@
         <v>567</v>
       </c>
       <c r="J149" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="K149" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
     </row>
     <row r="150" spans="1:11">
@@ -8547,10 +8547,10 @@
         <v>567</v>
       </c>
       <c r="J150" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="K150" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
     </row>
     <row r="151" spans="1:11">
@@ -8582,10 +8582,10 @@
         <v>567</v>
       </c>
       <c r="J151" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="K151" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
     </row>
     <row r="152" spans="1:11">
@@ -8617,10 +8617,10 @@
         <v>567</v>
       </c>
       <c r="J152" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="K152" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
     </row>
     <row r="153" spans="1:11">
@@ -8652,10 +8652,10 @@
         <v>567</v>
       </c>
       <c r="J153" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="K153" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
     </row>
     <row r="154" spans="1:11">
@@ -8687,10 +8687,10 @@
         <v>567</v>
       </c>
       <c r="J154" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="K154" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
     </row>
     <row r="155" spans="1:11">
@@ -8722,10 +8722,10 @@
         <v>567</v>
       </c>
       <c r="J155" t="s">
-        <v>568</v>
+        <v>590</v>
       </c>
       <c r="K155" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
     </row>
     <row r="156" spans="1:11">
@@ -8757,10 +8757,10 @@
         <v>567</v>
       </c>
       <c r="J156" t="s">
-        <v>568</v>
+        <v>619</v>
       </c>
       <c r="K156" t="s">
-        <v>619</v>
+        <v>569</v>
       </c>
     </row>
     <row r="157" spans="1:11">
@@ -8789,13 +8789,13 @@
         <v>566</v>
       </c>
       <c r="I157" t="s">
-        <v>567</v>
+        <v>623</v>
       </c>
       <c r="J157" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="K157" t="s">
-        <v>619</v>
+        <v>569</v>
       </c>
     </row>
     <row r="158" spans="1:11">
@@ -8827,10 +8827,10 @@
         <v>567</v>
       </c>
       <c r="J158" t="s">
-        <v>568</v>
+        <v>619</v>
       </c>
       <c r="K158" t="s">
-        <v>619</v>
+        <v>569</v>
       </c>
     </row>
     <row r="159" spans="1:11">
@@ -8862,10 +8862,10 @@
         <v>567</v>
       </c>
       <c r="J159" t="s">
-        <v>568</v>
+        <v>619</v>
       </c>
       <c r="K159" t="s">
-        <v>619</v>
+        <v>569</v>
       </c>
     </row>
     <row r="160" spans="1:11">
@@ -8897,10 +8897,10 @@
         <v>567</v>
       </c>
       <c r="J160" t="s">
-        <v>568</v>
+        <v>619</v>
       </c>
       <c r="K160" t="s">
-        <v>619</v>
+        <v>569</v>
       </c>
     </row>
     <row r="161" spans="1:11">
@@ -8932,10 +8932,10 @@
         <v>567</v>
       </c>
       <c r="J161" t="s">
-        <v>568</v>
+        <v>619</v>
       </c>
       <c r="K161" t="s">
-        <v>619</v>
+        <v>569</v>
       </c>
     </row>
     <row r="162" spans="1:11">
@@ -8967,10 +8967,10 @@
         <v>567</v>
       </c>
       <c r="J162" t="s">
-        <v>568</v>
+        <v>640</v>
       </c>
       <c r="K162" t="s">
-        <v>640</v>
+        <v>569</v>
       </c>
     </row>
     <row r="163" spans="1:11">
@@ -8999,13 +8999,13 @@
         <v>566</v>
       </c>
       <c r="I163" t="s">
-        <v>567</v>
+        <v>644</v>
       </c>
       <c r="J163" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="K163" t="s">
-        <v>645</v>
+        <v>569</v>
       </c>
     </row>
     <row r="164" spans="1:11">
@@ -9037,10 +9037,10 @@
         <v>567</v>
       </c>
       <c r="J164" t="s">
-        <v>568</v>
+        <v>650</v>
       </c>
       <c r="K164" t="s">
-        <v>650</v>
+        <v>569</v>
       </c>
     </row>
     <row r="165" spans="1:11">
@@ -9072,10 +9072,10 @@
         <v>567</v>
       </c>
       <c r="J165" t="s">
-        <v>568</v>
+        <v>650</v>
       </c>
       <c r="K165" t="s">
-        <v>650</v>
+        <v>569</v>
       </c>
     </row>
     <row r="166" spans="1:11">
@@ -9107,10 +9107,10 @@
         <v>567</v>
       </c>
       <c r="J166" t="s">
-        <v>568</v>
+        <v>650</v>
       </c>
       <c r="K166" t="s">
-        <v>650</v>
+        <v>569</v>
       </c>
     </row>
     <row r="167" spans="1:11">
@@ -9142,10 +9142,10 @@
         <v>567</v>
       </c>
       <c r="J167" t="s">
-        <v>568</v>
+        <v>650</v>
       </c>
       <c r="K167" t="s">
-        <v>650</v>
+        <v>569</v>
       </c>
     </row>
     <row r="168" spans="1:11">
@@ -9174,13 +9174,13 @@
         <v>566</v>
       </c>
       <c r="I168" t="s">
-        <v>567</v>
+        <v>663</v>
       </c>
       <c r="J168" t="s">
-        <v>663</v>
+        <v>650</v>
       </c>
       <c r="K168" t="s">
-        <v>650</v>
+        <v>569</v>
       </c>
     </row>
     <row r="169" spans="1:11">
@@ -9206,13 +9206,13 @@
         <v>566</v>
       </c>
       <c r="I169" t="s">
-        <v>567</v>
+        <v>663</v>
       </c>
       <c r="J169" t="s">
-        <v>663</v>
+        <v>650</v>
       </c>
       <c r="K169" t="s">
-        <v>650</v>
+        <v>569</v>
       </c>
     </row>
     <row r="170" spans="1:11">
@@ -9244,10 +9244,10 @@
         <v>567</v>
       </c>
       <c r="J170" t="s">
-        <v>568</v>
+        <v>650</v>
       </c>
       <c r="K170" t="s">
-        <v>650</v>
+        <v>569</v>
       </c>
     </row>
     <row r="171" spans="1:11">
@@ -9275,7 +9275,7 @@
       <c r="I171" t="s">
         <v>338</v>
       </c>
-      <c r="J171" t="s">
+      <c r="K171" t="s">
         <v>339</v>
       </c>
     </row>
@@ -9304,7 +9304,7 @@
       <c r="I172" t="s">
         <v>243</v>
       </c>
-      <c r="J172" t="s">
+      <c r="K172" t="s">
         <v>244</v>
       </c>
     </row>
@@ -9333,7 +9333,7 @@
       <c r="I173" t="s">
         <v>338</v>
       </c>
-      <c r="J173" t="s">
+      <c r="K173" t="s">
         <v>339</v>
       </c>
     </row>
@@ -9362,7 +9362,7 @@
       <c r="I174" t="s">
         <v>338</v>
       </c>
-      <c r="J174" t="s">
+      <c r="K174" t="s">
         <v>339</v>
       </c>
     </row>
@@ -9391,7 +9391,7 @@
       <c r="I175" t="s">
         <v>338</v>
       </c>
-      <c r="J175" t="s">
+      <c r="K175" t="s">
         <v>339</v>
       </c>
     </row>
@@ -9417,7 +9417,7 @@
       <c r="I176" t="s">
         <v>338</v>
       </c>
-      <c r="J176" t="s">
+      <c r="K176" t="s">
         <v>339</v>
       </c>
     </row>
@@ -9446,7 +9446,7 @@
       <c r="I177" t="s">
         <v>338</v>
       </c>
-      <c r="J177" t="s">
+      <c r="K177" t="s">
         <v>339</v>
       </c>
     </row>
@@ -9475,7 +9475,7 @@
       <c r="I178" t="s">
         <v>338</v>
       </c>
-      <c r="J178" t="s">
+      <c r="K178" t="s">
         <v>339</v>
       </c>
     </row>
@@ -9504,7 +9504,7 @@
       <c r="I179" t="s">
         <v>338</v>
       </c>
-      <c r="J179" t="s">
+      <c r="K179" t="s">
         <v>339</v>
       </c>
     </row>
@@ -9533,7 +9533,7 @@
       <c r="I180" t="s">
         <v>338</v>
       </c>
-      <c r="J180" t="s">
+      <c r="K180" t="s">
         <v>339</v>
       </c>
     </row>
@@ -9980,13 +9980,13 @@
         <v>707</v>
       </c>
       <c r="I193" t="s">
-        <v>575</v>
+        <v>746</v>
       </c>
       <c r="J193" t="s">
-        <v>746</v>
+        <v>709</v>
       </c>
       <c r="K193" t="s">
-        <v>710</v>
+        <v>576</v>
       </c>
     </row>
     <row r="194" spans="1:11">
@@ -10190,13 +10190,13 @@
         <v>707</v>
       </c>
       <c r="I199" t="s">
-        <v>708</v>
+        <v>766</v>
       </c>
       <c r="J199" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="K199" t="s">
-        <v>767</v>
+        <v>710</v>
       </c>
     </row>
     <row r="200" spans="1:11">
@@ -10225,13 +10225,13 @@
         <v>707</v>
       </c>
       <c r="I200" t="s">
-        <v>708</v>
+        <v>766</v>
       </c>
       <c r="J200" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="K200" t="s">
-        <v>767</v>
+        <v>710</v>
       </c>
     </row>
     <row r="201" spans="1:11">
@@ -10260,13 +10260,13 @@
         <v>707</v>
       </c>
       <c r="I201" t="s">
-        <v>708</v>
+        <v>766</v>
       </c>
       <c r="J201" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="K201" t="s">
-        <v>767</v>
+        <v>710</v>
       </c>
     </row>
     <row r="202" spans="1:11">
@@ -10292,13 +10292,13 @@
         <v>707</v>
       </c>
       <c r="I202" t="s">
-        <v>708</v>
+        <v>766</v>
       </c>
       <c r="J202" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="K202" t="s">
-        <v>767</v>
+        <v>710</v>
       </c>
     </row>
     <row r="203" spans="1:11">
@@ -10327,13 +10327,13 @@
         <v>707</v>
       </c>
       <c r="I203" t="s">
-        <v>575</v>
+        <v>746</v>
       </c>
       <c r="J203" t="s">
-        <v>746</v>
+        <v>767</v>
       </c>
       <c r="K203" t="s">
-        <v>767</v>
+        <v>576</v>
       </c>
     </row>
     <row r="204" spans="1:11">
@@ -10359,13 +10359,13 @@
         <v>707</v>
       </c>
       <c r="I204" t="s">
-        <v>708</v>
+        <v>766</v>
       </c>
       <c r="J204" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="K204" t="s">
-        <v>767</v>
+        <v>710</v>
       </c>
     </row>
     <row r="205" spans="1:11">
@@ -10394,13 +10394,13 @@
         <v>707</v>
       </c>
       <c r="I205" t="s">
-        <v>708</v>
+        <v>785</v>
       </c>
       <c r="J205" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="K205" t="s">
-        <v>786</v>
+        <v>710</v>
       </c>
     </row>
     <row r="206" spans="1:11">
@@ -10429,13 +10429,13 @@
         <v>707</v>
       </c>
       <c r="I206" t="s">
-        <v>708</v>
+        <v>785</v>
       </c>
       <c r="J206" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="K206" t="s">
-        <v>786</v>
+        <v>710</v>
       </c>
     </row>
     <row r="207" spans="1:11">
@@ -10461,13 +10461,13 @@
         <v>707</v>
       </c>
       <c r="I207" t="s">
-        <v>708</v>
+        <v>785</v>
       </c>
       <c r="J207" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="K207" t="s">
-        <v>786</v>
+        <v>710</v>
       </c>
     </row>
     <row r="208" spans="1:11">
@@ -10496,13 +10496,13 @@
         <v>707</v>
       </c>
       <c r="I208" t="s">
-        <v>575</v>
+        <v>746</v>
       </c>
       <c r="J208" t="s">
-        <v>746</v>
+        <v>786</v>
       </c>
       <c r="K208" t="s">
-        <v>786</v>
+        <v>576</v>
       </c>
     </row>
     <row r="209" spans="1:11">
@@ -10531,13 +10531,13 @@
         <v>707</v>
       </c>
       <c r="I209" t="s">
-        <v>708</v>
+        <v>785</v>
       </c>
       <c r="J209" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="K209" t="s">
-        <v>786</v>
+        <v>710</v>
       </c>
     </row>
     <row r="210" spans="1:11">
@@ -10735,13 +10735,13 @@
         <v>803</v>
       </c>
       <c r="I215" t="s">
-        <v>708</v>
+        <v>766</v>
       </c>
       <c r="J215" t="s">
-        <v>766</v>
+        <v>805</v>
       </c>
       <c r="K215" t="s">
-        <v>806</v>
+        <v>710</v>
       </c>
     </row>
     <row r="216" spans="1:11">
@@ -10904,13 +10904,13 @@
         <v>803</v>
       </c>
       <c r="I220" t="s">
-        <v>567</v>
+        <v>663</v>
       </c>
       <c r="J220" t="s">
-        <v>663</v>
+        <v>805</v>
       </c>
       <c r="K220" t="s">
-        <v>806</v>
+        <v>569</v>
       </c>
     </row>
     <row r="221" spans="1:11">
@@ -11114,10 +11114,10 @@
         <v>575</v>
       </c>
       <c r="J226" t="s">
+        <v>805</v>
+      </c>
+      <c r="K226" t="s">
         <v>576</v>
-      </c>
-      <c r="K226" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="227" spans="1:11">
@@ -11184,10 +11184,10 @@
         <v>338</v>
       </c>
       <c r="J228" t="s">
+        <v>805</v>
+      </c>
+      <c r="K228" t="s">
         <v>339</v>
-      </c>
-      <c r="K228" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="229" spans="1:11">
@@ -11216,13 +11216,13 @@
         <v>803</v>
       </c>
       <c r="I229" t="s">
-        <v>804</v>
+        <v>860</v>
       </c>
       <c r="J229" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="K229" t="s">
-        <v>861</v>
+        <v>806</v>
       </c>
     </row>
     <row r="230" spans="1:11">
@@ -11251,13 +11251,13 @@
         <v>803</v>
       </c>
       <c r="I230" t="s">
-        <v>804</v>
+        <v>860</v>
       </c>
       <c r="J230" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="K230" t="s">
-        <v>861</v>
+        <v>806</v>
       </c>
     </row>
     <row r="231" spans="1:11">
@@ -11286,13 +11286,13 @@
         <v>803</v>
       </c>
       <c r="I231" t="s">
-        <v>567</v>
+        <v>623</v>
       </c>
       <c r="J231" t="s">
-        <v>623</v>
+        <v>861</v>
       </c>
       <c r="K231" t="s">
-        <v>861</v>
+        <v>569</v>
       </c>
     </row>
     <row r="232" spans="1:11">
@@ -11321,13 +11321,13 @@
         <v>803</v>
       </c>
       <c r="I232" t="s">
-        <v>567</v>
+        <v>663</v>
       </c>
       <c r="J232" t="s">
-        <v>663</v>
+        <v>861</v>
       </c>
       <c r="K232" t="s">
-        <v>861</v>
+        <v>569</v>
       </c>
     </row>
     <row r="233" spans="1:11">
@@ -11356,13 +11356,13 @@
         <v>803</v>
       </c>
       <c r="I233" t="s">
-        <v>804</v>
+        <v>860</v>
       </c>
       <c r="J233" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="K233" t="s">
-        <v>861</v>
+        <v>806</v>
       </c>
     </row>
     <row r="234" spans="1:11">
@@ -11391,13 +11391,13 @@
         <v>803</v>
       </c>
       <c r="I234" t="s">
-        <v>804</v>
+        <v>860</v>
       </c>
       <c r="J234" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="K234" t="s">
-        <v>861</v>
+        <v>806</v>
       </c>
     </row>
     <row r="235" spans="1:11">
@@ -11426,13 +11426,13 @@
         <v>803</v>
       </c>
       <c r="I235" t="s">
-        <v>804</v>
+        <v>860</v>
       </c>
       <c r="J235" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="K235" t="s">
-        <v>861</v>
+        <v>806</v>
       </c>
     </row>
     <row r="236" spans="1:11">
@@ -11461,13 +11461,13 @@
         <v>803</v>
       </c>
       <c r="I236" t="s">
-        <v>804</v>
+        <v>860</v>
       </c>
       <c r="J236" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="K236" t="s">
-        <v>861</v>
+        <v>806</v>
       </c>
     </row>
     <row r="237" spans="1:11">
@@ -11496,13 +11496,13 @@
         <v>803</v>
       </c>
       <c r="I237" t="s">
-        <v>804</v>
+        <v>860</v>
       </c>
       <c r="J237" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="K237" t="s">
-        <v>861</v>
+        <v>806</v>
       </c>
     </row>
     <row r="238" spans="1:11">
@@ -11531,13 +11531,13 @@
         <v>803</v>
       </c>
       <c r="I238" t="s">
-        <v>804</v>
+        <v>860</v>
       </c>
       <c r="J238" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="K238" t="s">
-        <v>861</v>
+        <v>806</v>
       </c>
     </row>
     <row r="239" spans="1:11">
@@ -11566,13 +11566,13 @@
         <v>803</v>
       </c>
       <c r="I239" t="s">
-        <v>804</v>
+        <v>893</v>
       </c>
       <c r="J239" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="K239" t="s">
-        <v>894</v>
+        <v>806</v>
       </c>
     </row>
     <row r="240" spans="1:11">
@@ -11604,10 +11604,10 @@
         <v>338</v>
       </c>
       <c r="J240" t="s">
+        <v>900</v>
+      </c>
+      <c r="K240" t="s">
         <v>339</v>
-      </c>
-      <c r="K240" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="241" spans="1:11">
@@ -11639,10 +11639,10 @@
         <v>338</v>
       </c>
       <c r="J241" t="s">
+        <v>900</v>
+      </c>
+      <c r="K241" t="s">
         <v>339</v>
-      </c>
-      <c r="K241" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="242" spans="1:11">
@@ -11674,10 +11674,10 @@
         <v>338</v>
       </c>
       <c r="J242" t="s">
+        <v>900</v>
+      </c>
+      <c r="K242" t="s">
         <v>339</v>
-      </c>
-      <c r="K242" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="243" spans="1:11">
@@ -11709,10 +11709,10 @@
         <v>338</v>
       </c>
       <c r="J243" t="s">
+        <v>900</v>
+      </c>
+      <c r="K243" t="s">
         <v>339</v>
-      </c>
-      <c r="K243" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="244" spans="1:11">
@@ -11744,10 +11744,10 @@
         <v>338</v>
       </c>
       <c r="J244" t="s">
+        <v>900</v>
+      </c>
+      <c r="K244" t="s">
         <v>339</v>
-      </c>
-      <c r="K244" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="245" spans="1:11">
@@ -11779,10 +11779,10 @@
         <v>338</v>
       </c>
       <c r="J245" t="s">
+        <v>900</v>
+      </c>
+      <c r="K245" t="s">
         <v>339</v>
-      </c>
-      <c r="K245" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="246" spans="1:11">
@@ -11808,13 +11808,13 @@
         <v>899</v>
       </c>
       <c r="I246" t="s">
-        <v>533</v>
+        <v>919</v>
       </c>
       <c r="J246" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="K246" t="s">
-        <v>920</v>
+        <v>534</v>
       </c>
     </row>
     <row r="247" spans="1:11">
@@ -11842,7 +11842,7 @@
       <c r="I247" t="s">
         <v>197</v>
       </c>
-      <c r="J247" t="s">
+      <c r="K247" t="s">
         <v>198</v>
       </c>
     </row>
@@ -11871,7 +11871,7 @@
       <c r="I248" t="s">
         <v>197</v>
       </c>
-      <c r="J248" t="s">
+      <c r="K248" t="s">
         <v>198</v>
       </c>
     </row>
@@ -11900,7 +11900,7 @@
       <c r="I249" t="s">
         <v>932</v>
       </c>
-      <c r="J249" t="s">
+      <c r="K249" t="s">
         <v>933</v>
       </c>
     </row>
@@ -11929,7 +11929,7 @@
       <c r="I250" t="s">
         <v>197</v>
       </c>
-      <c r="J250" t="s">
+      <c r="K250" t="s">
         <v>198</v>
       </c>
     </row>
@@ -11955,7 +11955,7 @@
       <c r="I251" t="s">
         <v>197</v>
       </c>
-      <c r="J251" t="s">
+      <c r="K251" t="s">
         <v>198</v>
       </c>
     </row>
@@ -11984,7 +11984,7 @@
       <c r="I252" t="s">
         <v>197</v>
       </c>
-      <c r="J252" t="s">
+      <c r="K252" t="s">
         <v>198</v>
       </c>
     </row>
@@ -12010,7 +12010,7 @@
       <c r="I253" t="s">
         <v>946</v>
       </c>
-      <c r="J253" t="s">
+      <c r="K253" t="s">
         <v>947</v>
       </c>
     </row>
@@ -12039,7 +12039,7 @@
       <c r="I254" t="s">
         <v>454</v>
       </c>
-      <c r="J254" t="s">
+      <c r="K254" t="s">
         <v>455</v>
       </c>
     </row>
@@ -12068,7 +12068,7 @@
       <c r="I255" t="s">
         <v>954</v>
       </c>
-      <c r="J255" t="s">
+      <c r="K255" t="s">
         <v>955</v>
       </c>
     </row>
@@ -12097,11 +12097,11 @@
       <c r="I256" t="s">
         <v>954</v>
       </c>
-      <c r="J256" t="s">
+      <c r="K256" t="s">
         <v>955</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:11">
       <c r="A257" t="s">
         <v>959</v>
       </c>
@@ -12126,11 +12126,11 @@
       <c r="I257" t="s">
         <v>954</v>
       </c>
-      <c r="J257" t="s">
+      <c r="K257" t="s">
         <v>955</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:11">
       <c r="A258" t="s">
         <v>962</v>
       </c>
@@ -12155,11 +12155,11 @@
       <c r="I258" t="s">
         <v>708</v>
       </c>
-      <c r="J258" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="259" spans="1:10">
+      <c r="K258" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11">
       <c r="A259" t="s">
         <v>965</v>
       </c>
@@ -12184,11 +12184,11 @@
       <c r="I259" t="s">
         <v>954</v>
       </c>
-      <c r="J259" t="s">
+      <c r="K259" t="s">
         <v>955</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:11">
       <c r="A260" t="s">
         <v>967</v>
       </c>
@@ -12213,11 +12213,11 @@
       <c r="I260" t="s">
         <v>338</v>
       </c>
-      <c r="J260" t="s">
+      <c r="K260" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:11">
       <c r="A261" t="s">
         <v>970</v>
       </c>
@@ -12242,11 +12242,11 @@
       <c r="I261" t="s">
         <v>973</v>
       </c>
-      <c r="J261" t="s">
+      <c r="K261" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:11">
       <c r="A262" t="s">
         <v>975</v>
       </c>
@@ -12271,11 +12271,11 @@
       <c r="I262" t="s">
         <v>338</v>
       </c>
-      <c r="J262" t="s">
+      <c r="K262" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:11">
       <c r="A263" t="s">
         <v>978</v>
       </c>
@@ -12300,11 +12300,11 @@
       <c r="I263" t="s">
         <v>981</v>
       </c>
-      <c r="J263" t="s">
+      <c r="K263" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:11">
       <c r="A264" t="s">
         <v>983</v>
       </c>
@@ -12329,11 +12329,11 @@
       <c r="I264" t="s">
         <v>59</v>
       </c>
-      <c r="J264" t="s">
+      <c r="K264" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:11">
       <c r="A265" t="s">
         <v>986</v>
       </c>
@@ -12358,11 +12358,11 @@
       <c r="I265" t="s">
         <v>19</v>
       </c>
-      <c r="J265" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="266" spans="1:10">
+      <c r="K265" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11">
       <c r="A266" t="s">
         <v>989</v>
       </c>
@@ -12387,11 +12387,11 @@
       <c r="I266" t="s">
         <v>992</v>
       </c>
-      <c r="J266" t="s">
+      <c r="K266" t="s">
         <v>993</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:11">
       <c r="A267" t="s">
         <v>994</v>
       </c>
@@ -12416,11 +12416,11 @@
       <c r="I267" t="s">
         <v>243</v>
       </c>
-      <c r="J267" t="s">
+      <c r="K267" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:11">
       <c r="A268" t="s">
         <v>999</v>
       </c>
@@ -12445,11 +12445,11 @@
       <c r="I268" t="s">
         <v>422</v>
       </c>
-      <c r="J268" t="s">
+      <c r="K268" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:11">
       <c r="A269" t="s">
         <v>1004</v>
       </c>
@@ -12474,11 +12474,11 @@
       <c r="I269" t="s">
         <v>243</v>
       </c>
-      <c r="J269" t="s">
+      <c r="K269" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:11">
       <c r="A270" t="s">
         <v>1009</v>
       </c>
@@ -12503,11 +12503,11 @@
       <c r="I270" t="s">
         <v>243</v>
       </c>
-      <c r="J270" t="s">
+      <c r="K270" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:11">
       <c r="A271" t="s">
         <v>1012</v>
       </c>
@@ -12532,11 +12532,11 @@
       <c r="I271" t="s">
         <v>1017</v>
       </c>
-      <c r="J271" t="s">
+      <c r="K271" t="s">
         <v>1018</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:11">
       <c r="A272" t="s">
         <v>1019</v>
       </c>
@@ -12558,11 +12558,11 @@
       <c r="I272" t="s">
         <v>1017</v>
       </c>
-      <c r="J272" t="s">
+      <c r="K272" t="s">
         <v>1018</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:11">
       <c r="A273" t="s">
         <v>1021</v>
       </c>
@@ -12587,11 +12587,11 @@
       <c r="I273" t="s">
         <v>1017</v>
       </c>
-      <c r="J273" t="s">
+      <c r="K273" t="s">
         <v>1018</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:11">
       <c r="A274" t="s">
         <v>1024</v>
       </c>
@@ -12613,11 +12613,11 @@
       <c r="I274" t="s">
         <v>1017</v>
       </c>
-      <c r="J274" t="s">
+      <c r="K274" t="s">
         <v>1018</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:11">
       <c r="A275" t="s">
         <v>1026</v>
       </c>
@@ -12642,11 +12642,11 @@
       <c r="I275" t="s">
         <v>1017</v>
       </c>
-      <c r="J275" t="s">
+      <c r="K275" t="s">
         <v>1018</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:11">
       <c r="A276" t="s">
         <v>1029</v>
       </c>
@@ -12671,11 +12671,11 @@
       <c r="I276" t="s">
         <v>1017</v>
       </c>
-      <c r="J276" t="s">
+      <c r="K276" t="s">
         <v>1018</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:11">
       <c r="A277" t="s">
         <v>1032</v>
       </c>
@@ -12700,11 +12700,11 @@
       <c r="I277" t="s">
         <v>1017</v>
       </c>
-      <c r="J277" t="s">
+      <c r="K277" t="s">
         <v>1018</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:11">
       <c r="A278" t="s">
         <v>1035</v>
       </c>
@@ -12729,11 +12729,11 @@
       <c r="I278" t="s">
         <v>422</v>
       </c>
-      <c r="J278" t="s">
+      <c r="K278" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:11">
       <c r="A279" t="s">
         <v>1040</v>
       </c>
@@ -12758,11 +12758,11 @@
       <c r="I279" t="s">
         <v>95</v>
       </c>
-      <c r="J279" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="280" spans="1:10">
+      <c r="K279" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11">
       <c r="A280" t="s">
         <v>1043</v>
       </c>
@@ -12787,11 +12787,11 @@
       <c r="I280" t="s">
         <v>19</v>
       </c>
-      <c r="J280" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="281" spans="1:10">
+      <c r="K280" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11">
       <c r="A281" t="s">
         <v>1046</v>
       </c>
@@ -12816,11 +12816,11 @@
       <c r="I281" t="s">
         <v>352</v>
       </c>
-      <c r="J281" t="s">
+      <c r="K281" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:11">
       <c r="A282" t="s">
         <v>1049</v>
       </c>
@@ -12845,11 +12845,11 @@
       <c r="I282" t="s">
         <v>254</v>
       </c>
-      <c r="J282" t="s">
+      <c r="K282" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:11">
       <c r="A283" t="s">
         <v>1052</v>
       </c>
@@ -12872,13 +12872,13 @@
         <v>1056</v>
       </c>
       <c r="I283" t="s">
-        <v>804</v>
-      </c>
-      <c r="J283" t="s">
         <v>893</v>
       </c>
-    </row>
-    <row r="284" spans="1:10">
+      <c r="K283" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11">
       <c r="A284" t="s">
         <v>1057</v>
       </c>
@@ -12903,11 +12903,11 @@
       <c r="I284" t="s">
         <v>254</v>
       </c>
-      <c r="J284" t="s">
+      <c r="K284" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:11">
       <c r="A285" t="s">
         <v>1062</v>
       </c>
@@ -12929,11 +12929,11 @@
       <c r="I285" t="s">
         <v>352</v>
       </c>
-      <c r="J285" t="s">
+      <c r="K285" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:11">
       <c r="A286" t="s">
         <v>1066</v>
       </c>
@@ -12958,11 +12958,11 @@
       <c r="I286" t="s">
         <v>981</v>
       </c>
-      <c r="J286" t="s">
+      <c r="K286" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:11">
       <c r="A287" t="s">
         <v>1071</v>
       </c>
@@ -12987,11 +12987,11 @@
       <c r="I287" t="s">
         <v>981</v>
       </c>
-      <c r="J287" t="s">
+      <c r="K287" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:11">
       <c r="A288" t="s">
         <v>1074</v>
       </c>
@@ -13016,11 +13016,11 @@
       <c r="I288" t="s">
         <v>75</v>
       </c>
-      <c r="J288" t="s">
+      <c r="K288" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:11">
       <c r="A289" t="s">
         <v>1077</v>
       </c>
@@ -13045,11 +13045,11 @@
       <c r="I289" t="s">
         <v>59</v>
       </c>
-      <c r="J289" t="s">
+      <c r="K289" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:11">
       <c r="A290" t="s">
         <v>1080</v>
       </c>
@@ -13074,11 +13074,11 @@
       <c r="I290" t="s">
         <v>59</v>
       </c>
-      <c r="J290" t="s">
+      <c r="K290" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:11">
       <c r="A291" t="s">
         <v>1083</v>
       </c>
@@ -13103,11 +13103,11 @@
       <c r="I291" t="s">
         <v>352</v>
       </c>
-      <c r="J291" t="s">
+      <c r="K291" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="292" spans="1:10">
+    <row r="292" spans="1:11">
       <c r="A292" t="s">
         <v>1086</v>
       </c>
@@ -13132,11 +13132,11 @@
       <c r="I292" t="s">
         <v>352</v>
       </c>
-      <c r="J292" t="s">
+      <c r="K292" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="293" spans="1:10">
+    <row r="293" spans="1:11">
       <c r="A293" t="s">
         <v>1089</v>
       </c>
@@ -13161,11 +13161,11 @@
       <c r="I293" t="s">
         <v>352</v>
       </c>
-      <c r="J293" t="s">
+      <c r="K293" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="294" spans="1:10">
+    <row r="294" spans="1:11">
       <c r="A294" t="s">
         <v>1092</v>
       </c>
@@ -13190,11 +13190,11 @@
       <c r="I294" t="s">
         <v>352</v>
       </c>
-      <c r="J294" t="s">
+      <c r="K294" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="295" spans="1:10">
+    <row r="295" spans="1:11">
       <c r="A295" t="s">
         <v>1095</v>
       </c>
@@ -13219,11 +13219,11 @@
       <c r="I295" t="s">
         <v>352</v>
       </c>
-      <c r="J295" t="s">
+      <c r="K295" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="296" spans="1:10">
+    <row r="296" spans="1:11">
       <c r="A296" t="s">
         <v>1100</v>
       </c>
@@ -13248,7 +13248,7 @@
       <c r="I296" t="s">
         <v>352</v>
       </c>
-      <c r="J296" t="s">
+      <c r="K296" t="s">
         <v>353</v>
       </c>
     </row>

</xml_diff>